<commit_message>
added 4 accounts, added schedule functions
</commit_message>
<xml_diff>
--- a/email-blacklist.xlsx
+++ b/email-blacklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Learning/Coding/Python3/email-filter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD970993-55D5-544B-AB61-05F504D300E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A20D3E9-A9B0-FF4F-9916-355984F565AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5400" windowWidth="19140" windowHeight="12320" xr2:uid="{9EAAAB48-0564-264C-871F-A0757B4CA22E}"/>
   </bookViews>
@@ -38,10 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>test@gmail.com</t>
+    <t>Email Black List</t>
   </si>
   <si>
-    <t>Email Black List</t>
+    <t>test@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -404,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5007EC2-9EFF-F74B-A6A4-12B805195642}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -417,20 +417,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{D71C30EC-95B3-9E40-8F46-323ADC50C3EE}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{0CFCEA9B-6450-0F4A-B1F4-F38628BBBB36}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>